<commit_message>
EPBDS-9041 fix Comparison_qe tests for primitives
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Comparison_eq.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Comparison_eq.xlsx
@@ -1,15 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvlad\.openl-webstudio\user-workspace\admin\EPBDS-9041_6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867D8DFE-3A7A-43DE-9CF7-4E30A956D3DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EQ" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1825,7 +1839,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1849,7 +1863,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1859,6 +1873,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1907,7 +1927,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1930,11 +1950,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="ACT_H" xfId="2"/>
+    <cellStyle name="ACT_H" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1992,7 +2013,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2025,9 +2046,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2060,6 +2098,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2235,39 +2290,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AE381"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C356" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F372" sqref="F372"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="2.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="17.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="18.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="18.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="2.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="18.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="17.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="18.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="20" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="19.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="21.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="31" width="9.140625" style="1"/>
-    <col min="32" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="25" max="25" width="20.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="21.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="31" width="9.109375" style="1"/>
+    <col min="32" max="16384" width="9.109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="11" t="s">
         <v>114</v>
       </c>
@@ -2295,7 +2352,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
         <v>0</v>
@@ -2367,7 +2424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
@@ -2441,7 +2498,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>75</v>
       </c>
@@ -2541,7 +2598,7 @@
         <v>= $X$b1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
@@ -2637,7 +2694,7 @@
         <v>= $X$s1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
@@ -2733,7 +2790,7 @@
         <v>= $X$i1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2829,7 +2886,7 @@
         <v>= $X$l1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2925,7 +2982,7 @@
         <v>= $X$f1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
@@ -3021,7 +3078,7 @@
         <v>= $X$d1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="C12" s="1" t="s">
         <v>37</v>
@@ -3118,7 +3175,7 @@
         <v>= $X$B1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
@@ -3214,7 +3271,7 @@
         <v>= $X$S1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
@@ -3310,7 +3367,7 @@
         <v>= $X$I1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
@@ -3406,7 +3463,7 @@
         <v>= $X$L1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
@@ -3502,7 +3559,7 @@
         <v>= $X$F1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
@@ -3598,7 +3655,7 @@
         <v>= $X$D1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>43</v>
       </c>
@@ -3694,7 +3751,7 @@
         <v>= $X$BI1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
@@ -3790,7 +3847,7 @@
         <v>= $X$BD1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="20" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
@@ -3886,7 +3943,7 @@
         <v>= $X$BV1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
@@ -3982,7 +4039,7 @@
         <v>= $X$SV1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="22" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>47</v>
       </c>
@@ -4078,7 +4135,7 @@
         <v>= $X$IV1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="23" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
@@ -4174,7 +4231,7 @@
         <v>= $X$LV1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="24" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
@@ -4270,7 +4327,7 @@
         <v>= $X$FV1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="25" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>50</v>
       </c>
@@ -4366,7 +4423,7 @@
         <v>= $X$DV1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
@@ -4462,7 +4519,7 @@
         <v>= $X$BIV1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
@@ -4558,7 +4615,7 @@
         <v>= $X$BDV1 == $BDV2$Y</v>
       </c>
     </row>
-    <row r="33" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C33" s="10" t="s">
         <v>141</v>
       </c>
@@ -4588,7 +4645,7 @@
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
     </row>
-    <row r="34" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C34" s="6" t="s">
         <v>53</v>
       </c>
@@ -4662,7 +4719,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
         <v>55</v>
       </c>
@@ -4736,7 +4793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C36" s="7">
         <v>1</v>
       </c>
@@ -4810,7 +4867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C37" s="7">
         <v>-1</v>
       </c>
@@ -4884,7 +4941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C38" s="6">
         <v>0</v>
       </c>
@@ -4958,7 +5015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C39" s="6">
         <v>-15</v>
       </c>
@@ -5032,7 +5089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C40" s="6">
         <v>-15</v>
       </c>
@@ -5106,7 +5163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C41" s="6"/>
       <c r="D41" s="8"/>
       <c r="E41" s="6" t="b">
@@ -5127,56 +5184,56 @@
       <c r="J41" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="K41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="X41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z41" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="W41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C42" s="6">
         <v>15</v>
       </c>
@@ -5248,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C43" s="6"/>
       <c r="D43" s="8">
         <v>15</v>
@@ -5320,7 +5377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C44" s="6">
         <v>15</v>
       </c>
@@ -5394,7 +5451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C45" s="6">
         <v>-3</v>
       </c>
@@ -5468,7 +5525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C49" s="10" t="s">
         <v>142</v>
       </c>
@@ -5498,7 +5555,7 @@
       <c r="Y49" s="6"/>
       <c r="Z49" s="6"/>
     </row>
-    <row r="50" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C50" s="6" t="s">
         <v>53</v>
       </c>
@@ -5572,7 +5629,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C51" s="6" t="s">
         <v>55</v>
       </c>
@@ -5646,7 +5703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C52" s="7">
         <v>1</v>
       </c>
@@ -5720,7 +5777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C53" s="7">
         <v>-1</v>
       </c>
@@ -5794,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C54" s="6">
         <v>0</v>
       </c>
@@ -5868,7 +5925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C55" s="6">
         <v>-15</v>
       </c>
@@ -5942,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C56" s="6">
         <v>-15</v>
       </c>
@@ -6016,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C57" s="6"/>
       <c r="D57" s="8"/>
       <c r="E57" s="6" t="b">
@@ -6037,56 +6094,56 @@
       <c r="J57" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="K57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="X57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z57" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="W57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C58" s="6">
         <v>15</v>
       </c>
@@ -6158,7 +6215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C59" s="6"/>
       <c r="D59" s="8">
         <v>15</v>
@@ -6230,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C60" s="6">
         <v>15</v>
       </c>
@@ -6304,7 +6361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C61" s="6">
         <v>-3</v>
       </c>
@@ -6378,7 +6435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C65" s="10" t="s">
         <v>143</v>
       </c>
@@ -6408,7 +6465,7 @@
       <c r="Y65" s="6"/>
       <c r="Z65" s="6"/>
     </row>
-    <row r="66" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C66" s="6" t="s">
         <v>53</v>
       </c>
@@ -6482,7 +6539,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C67" s="6" t="s">
         <v>55</v>
       </c>
@@ -6556,7 +6613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C68" s="7">
         <v>1</v>
       </c>
@@ -6630,7 +6687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C69" s="7">
         <v>-1</v>
       </c>
@@ -6704,7 +6761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C70" s="6">
         <v>0</v>
       </c>
@@ -6778,7 +6835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C71" s="6">
         <v>-15</v>
       </c>
@@ -6852,7 +6909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C72" s="6">
         <v>-15</v>
       </c>
@@ -6926,7 +6983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C73" s="6"/>
       <c r="D73" s="8"/>
       <c r="E73" s="6" t="b">
@@ -6947,56 +7004,56 @@
       <c r="J73" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="K73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="X73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z73" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="W73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z73" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C74" s="6">
         <v>15</v>
       </c>
@@ -7068,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C75" s="6"/>
       <c r="D75" s="8">
         <v>15</v>
@@ -7140,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C76" s="6">
         <v>15</v>
       </c>
@@ -7214,7 +7271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C77" s="6">
         <v>-3</v>
       </c>
@@ -7288,7 +7345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C81" s="10" t="s">
         <v>166</v>
       </c>
@@ -7318,7 +7375,7 @@
       <c r="Y81" s="6"/>
       <c r="Z81" s="6"/>
     </row>
-    <row r="82" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C82" s="6" t="s">
         <v>53</v>
       </c>
@@ -7392,7 +7449,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C83" s="6" t="s">
         <v>55</v>
       </c>
@@ -7466,7 +7523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C84" s="7">
         <v>1</v>
       </c>
@@ -7540,7 +7597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C85" s="7">
         <v>-1</v>
       </c>
@@ -7614,7 +7671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C86" s="6">
         <v>0</v>
       </c>
@@ -7688,7 +7745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C87" s="6">
         <v>-15</v>
       </c>
@@ -7762,7 +7819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C88" s="6">
         <v>-15</v>
       </c>
@@ -7836,7 +7893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C89" s="6"/>
       <c r="D89" s="8"/>
       <c r="E89" s="6" t="b">
@@ -7857,56 +7914,56 @@
       <c r="J89" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="K89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="X89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z89" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="W89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z89" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C90" s="6">
         <v>15</v>
       </c>
@@ -7978,7 +8035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C91" s="6"/>
       <c r="D91" s="8">
         <v>15</v>
@@ -8050,7 +8107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C92" s="6">
         <v>15</v>
       </c>
@@ -8124,7 +8181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C93" s="6">
         <v>-3</v>
       </c>
@@ -8198,7 +8255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C97" s="10" t="s">
         <v>189</v>
       </c>
@@ -8228,7 +8285,7 @@
       <c r="Y97" s="6"/>
       <c r="Z97" s="6"/>
     </row>
-    <row r="98" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C98" s="6" t="s">
         <v>53</v>
       </c>
@@ -8302,7 +8359,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="99" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C99" s="6" t="s">
         <v>55</v>
       </c>
@@ -8376,7 +8433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C100" s="7">
         <v>1</v>
       </c>
@@ -8450,7 +8507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C101" s="7">
         <v>-1</v>
       </c>
@@ -8524,7 +8581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C102" s="6">
         <v>0</v>
       </c>
@@ -8598,7 +8655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C103" s="6">
         <v>-15</v>
       </c>
@@ -8672,7 +8729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C104" s="6">
         <v>-15</v>
       </c>
@@ -8746,7 +8803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C105" s="6"/>
       <c r="D105" s="8"/>
       <c r="E105" s="6" t="b">
@@ -8767,56 +8824,56 @@
       <c r="J105" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="K105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="X105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y105" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z105" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="W105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z105" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C106" s="6">
         <v>15</v>
       </c>
@@ -8888,7 +8945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C107" s="6"/>
       <c r="D107" s="8">
         <v>15</v>
@@ -8960,7 +9017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C108" s="6">
         <v>15</v>
       </c>
@@ -9034,7 +9091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C109" s="6">
         <v>-3</v>
       </c>
@@ -9108,7 +9165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C113" s="10" t="s">
         <v>211</v>
       </c>
@@ -9138,7 +9195,7 @@
       <c r="Y113" s="6"/>
       <c r="Z113" s="6"/>
     </row>
-    <row r="114" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C114" s="6" t="s">
         <v>53</v>
       </c>
@@ -9212,7 +9269,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="115" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C115" s="6" t="s">
         <v>55</v>
       </c>
@@ -9286,7 +9343,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C116" s="7">
         <v>1</v>
       </c>
@@ -9360,7 +9417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C117" s="7">
         <v>-1</v>
       </c>
@@ -9434,7 +9491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C118" s="6">
         <v>0</v>
       </c>
@@ -9508,7 +9565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C119" s="6">
         <v>-15</v>
       </c>
@@ -9582,7 +9639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C120" s="6">
         <v>-15</v>
       </c>
@@ -9656,7 +9713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C121" s="6"/>
       <c r="D121" s="8"/>
       <c r="E121" s="6" t="b">
@@ -9677,56 +9734,56 @@
       <c r="J121" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="K121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="X121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y121" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z121" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="W121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z121" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C122" s="6">
         <v>15</v>
       </c>
@@ -9798,7 +9855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C123" s="6"/>
       <c r="D123" s="8">
         <v>15</v>
@@ -9870,7 +9927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C124" s="6">
         <v>15</v>
       </c>
@@ -9944,7 +10001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C125" s="6">
         <v>-3</v>
       </c>
@@ -10018,7 +10075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C129" s="10" t="s">
         <v>234</v>
       </c>
@@ -10048,7 +10105,7 @@
       <c r="Y129" s="6"/>
       <c r="Z129" s="6"/>
     </row>
-    <row r="130" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C130" s="6" t="s">
         <v>53</v>
       </c>
@@ -10122,7 +10179,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="131" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C131" s="6" t="s">
         <v>55</v>
       </c>
@@ -10196,7 +10253,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C132" s="7">
         <v>1</v>
       </c>
@@ -10270,7 +10327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C133" s="7">
         <v>-1</v>
       </c>
@@ -10344,7 +10401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C134" s="6">
         <v>0</v>
       </c>
@@ -10418,7 +10475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C135" s="6">
         <v>-15</v>
       </c>
@@ -10492,7 +10549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C136" s="6">
         <v>-15</v>
       </c>
@@ -10566,26 +10623,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C137" s="6"/>
       <c r="D137" s="8"/>
-      <c r="E137" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F137" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G137" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H137" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I137" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J137" s="6" t="b">
-        <v>1</v>
+      <c r="E137" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F137" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G137" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H137" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I137" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J137" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K137" s="6" t="b">
         <v>1</v>
@@ -10636,7 +10693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C138" s="6">
         <v>15</v>
       </c>
@@ -10708,7 +10765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C139" s="6"/>
       <c r="D139" s="8">
         <v>15</v>
@@ -10780,7 +10837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C140" s="6">
         <v>15</v>
       </c>
@@ -10854,7 +10911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C141" s="6">
         <v>-3</v>
       </c>
@@ -10928,7 +10985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C145" s="10" t="s">
         <v>257</v>
       </c>
@@ -10958,7 +11015,7 @@
       <c r="Y145" s="6"/>
       <c r="Z145" s="6"/>
     </row>
-    <row r="146" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C146" s="6" t="s">
         <v>53</v>
       </c>
@@ -11032,7 +11089,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="147" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C147" s="6" t="s">
         <v>55</v>
       </c>
@@ -11106,7 +11163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="148" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C148" s="7">
         <v>1</v>
       </c>
@@ -11180,7 +11237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C149" s="7">
         <v>-1</v>
       </c>
@@ -11254,7 +11311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C150" s="6">
         <v>0</v>
       </c>
@@ -11328,7 +11385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C151" s="6">
         <v>-15</v>
       </c>
@@ -11402,7 +11459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C152" s="6">
         <v>-15</v>
       </c>
@@ -11476,26 +11533,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C153" s="6"/>
       <c r="D153" s="8"/>
-      <c r="E153" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F153" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G153" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H153" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I153" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J153" s="6" t="b">
-        <v>1</v>
+      <c r="E153" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F153" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G153" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H153" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I153" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J153" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K153" s="6" t="b">
         <v>1</v>
@@ -11546,7 +11603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C154" s="6">
         <v>15</v>
       </c>
@@ -11618,7 +11675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C155" s="6"/>
       <c r="D155" s="8">
         <v>15</v>
@@ -11690,7 +11747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C156" s="6">
         <v>15</v>
       </c>
@@ -11764,7 +11821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C157" s="6">
         <v>-3</v>
       </c>
@@ -11838,7 +11895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C161" s="10" t="s">
         <v>280</v>
       </c>
@@ -11868,7 +11925,7 @@
       <c r="Y161" s="6"/>
       <c r="Z161" s="6"/>
     </row>
-    <row r="162" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C162" s="6" t="s">
         <v>53</v>
       </c>
@@ -11942,7 +11999,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="163" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C163" s="6" t="s">
         <v>55</v>
       </c>
@@ -12016,7 +12073,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="164" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C164" s="7">
         <v>1</v>
       </c>
@@ -12090,7 +12147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C165" s="7">
         <v>-1</v>
       </c>
@@ -12164,7 +12221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C166" s="6">
         <v>0</v>
       </c>
@@ -12238,7 +12295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C167" s="6">
         <v>-15</v>
       </c>
@@ -12312,7 +12369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C168" s="6">
         <v>-15</v>
       </c>
@@ -12386,26 +12443,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C169" s="6"/>
       <c r="D169" s="8"/>
-      <c r="E169" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F169" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G169" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H169" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I169" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J169" s="6" t="b">
-        <v>1</v>
+      <c r="E169" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F169" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G169" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H169" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I169" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J169" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K169" s="6" t="b">
         <v>1</v>
@@ -12456,7 +12513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C170" s="6">
         <v>15</v>
       </c>
@@ -12528,7 +12585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C171" s="6"/>
       <c r="D171" s="8">
         <v>15</v>
@@ -12600,7 +12657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C172" s="6">
         <v>15</v>
       </c>
@@ -12674,7 +12731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C173" s="6">
         <v>-3</v>
       </c>
@@ -12748,7 +12805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C177" s="10" t="s">
         <v>303</v>
       </c>
@@ -12778,7 +12835,7 @@
       <c r="Y177" s="6"/>
       <c r="Z177" s="6"/>
     </row>
-    <row r="178" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C178" s="6" t="s">
         <v>53</v>
       </c>
@@ -12852,7 +12909,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="179" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C179" s="6" t="s">
         <v>55</v>
       </c>
@@ -12926,7 +12983,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="180" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C180" s="7">
         <v>1</v>
       </c>
@@ -13000,7 +13057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C181" s="7">
         <v>-1</v>
       </c>
@@ -13074,7 +13131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C182" s="6">
         <v>0</v>
       </c>
@@ -13148,7 +13205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C183" s="6">
         <v>-15</v>
       </c>
@@ -13222,7 +13279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C184" s="6">
         <v>-15</v>
       </c>
@@ -13296,26 +13353,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C185" s="6"/>
       <c r="D185" s="8"/>
-      <c r="E185" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F185" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G185" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H185" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I185" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J185" s="6" t="b">
-        <v>1</v>
+      <c r="E185" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F185" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G185" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H185" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I185" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J185" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K185" s="6" t="b">
         <v>1</v>
@@ -13366,7 +13423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C186" s="6">
         <v>15</v>
       </c>
@@ -13438,7 +13495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C187" s="6"/>
       <c r="D187" s="8">
         <v>15</v>
@@ -13510,7 +13567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C188" s="6">
         <v>15</v>
       </c>
@@ -13584,7 +13641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C189" s="6">
         <v>-3</v>
       </c>
@@ -13658,7 +13715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C193" s="10" t="s">
         <v>326</v>
       </c>
@@ -13688,7 +13745,7 @@
       <c r="Y193" s="6"/>
       <c r="Z193" s="6"/>
     </row>
-    <row r="194" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C194" s="6" t="s">
         <v>53</v>
       </c>
@@ -13762,7 +13819,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="195" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C195" s="6" t="s">
         <v>55</v>
       </c>
@@ -13836,7 +13893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C196" s="7">
         <v>1</v>
       </c>
@@ -13910,7 +13967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C197" s="7">
         <v>-1</v>
       </c>
@@ -13984,7 +14041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C198" s="6">
         <v>0</v>
       </c>
@@ -14058,7 +14115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C199" s="6">
         <v>-15</v>
       </c>
@@ -14132,7 +14189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C200" s="6">
         <v>-15</v>
       </c>
@@ -14206,26 +14263,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C201" s="6"/>
       <c r="D201" s="8"/>
-      <c r="E201" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F201" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G201" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H201" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I201" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J201" s="6" t="b">
-        <v>1</v>
+      <c r="E201" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F201" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G201" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H201" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I201" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J201" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K201" s="6" t="b">
         <v>1</v>
@@ -14276,7 +14333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C202" s="6">
         <v>15</v>
       </c>
@@ -14348,7 +14405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C203" s="6"/>
       <c r="D203" s="8">
         <v>15</v>
@@ -14420,7 +14477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C204" s="6">
         <v>15</v>
       </c>
@@ -14494,7 +14551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C205" s="6">
         <v>-3</v>
       </c>
@@ -14568,7 +14625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C209" s="10" t="s">
         <v>349</v>
       </c>
@@ -14598,7 +14655,7 @@
       <c r="Y209" s="6"/>
       <c r="Z209" s="6"/>
     </row>
-    <row r="210" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C210" s="6" t="s">
         <v>53</v>
       </c>
@@ -14672,7 +14729,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="211" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C211" s="6" t="s">
         <v>55</v>
       </c>
@@ -14746,7 +14803,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="212" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C212" s="7">
         <v>1</v>
       </c>
@@ -14820,7 +14877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C213" s="7">
         <v>-1</v>
       </c>
@@ -14894,7 +14951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C214" s="6">
         <v>0</v>
       </c>
@@ -14968,7 +15025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C215" s="6">
         <v>-15</v>
       </c>
@@ -15042,7 +15099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C216" s="6">
         <v>-15</v>
       </c>
@@ -15116,26 +15173,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C217" s="6"/>
       <c r="D217" s="8"/>
-      <c r="E217" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F217" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G217" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H217" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I217" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J217" s="6" t="b">
-        <v>1</v>
+      <c r="E217" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F217" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G217" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H217" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I217" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J217" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K217" s="6" t="b">
         <v>1</v>
@@ -15186,7 +15243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C218" s="6">
         <v>15</v>
       </c>
@@ -15258,7 +15315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C219" s="6"/>
       <c r="D219" s="8">
         <v>15</v>
@@ -15330,7 +15387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C220" s="6">
         <v>15</v>
       </c>
@@ -15404,7 +15461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C221" s="6">
         <v>-3</v>
       </c>
@@ -15478,7 +15535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C225" s="10" t="s">
         <v>372</v>
       </c>
@@ -15508,7 +15565,7 @@
       <c r="Y225" s="6"/>
       <c r="Z225" s="6"/>
     </row>
-    <row r="226" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C226" s="6" t="s">
         <v>53</v>
       </c>
@@ -15582,7 +15639,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="227" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C227" s="6" t="s">
         <v>55</v>
       </c>
@@ -15656,7 +15713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="228" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C228" s="7">
         <v>1</v>
       </c>
@@ -15730,7 +15787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C229" s="7">
         <v>-1</v>
       </c>
@@ -15804,7 +15861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C230" s="6">
         <v>0</v>
       </c>
@@ -15878,7 +15935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C231" s="6">
         <v>-15</v>
       </c>
@@ -15952,7 +16009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C232" s="6">
         <v>-15</v>
       </c>
@@ -16026,26 +16083,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C233" s="6"/>
       <c r="D233" s="8"/>
-      <c r="E233" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F233" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G233" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H233" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I233" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J233" s="6" t="b">
-        <v>1</v>
+      <c r="E233" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F233" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G233" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H233" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I233" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J233" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K233" s="6" t="b">
         <v>1</v>
@@ -16096,7 +16153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C234" s="6">
         <v>15</v>
       </c>
@@ -16168,7 +16225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="235" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C235" s="6"/>
       <c r="D235" s="8">
         <v>15</v>
@@ -16240,7 +16297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="236" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C236" s="6">
         <v>15</v>
       </c>
@@ -16314,7 +16371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="237" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C237" s="6">
         <v>-3</v>
       </c>
@@ -16388,7 +16445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="241" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C241" s="10" t="s">
         <v>395</v>
       </c>
@@ -16418,7 +16475,7 @@
       <c r="Y241" s="6"/>
       <c r="Z241" s="6"/>
     </row>
-    <row r="242" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="242" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C242" s="6" t="s">
         <v>53</v>
       </c>
@@ -16492,7 +16549,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="243" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="243" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C243" s="6" t="s">
         <v>55</v>
       </c>
@@ -16566,7 +16623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="244" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C244" s="7">
         <v>1</v>
       </c>
@@ -16640,7 +16697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="245" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C245" s="7">
         <v>-1</v>
       </c>
@@ -16714,7 +16771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="246" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C246" s="6">
         <v>0</v>
       </c>
@@ -16788,7 +16845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="247" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C247" s="6">
         <v>-15</v>
       </c>
@@ -16862,7 +16919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="248" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C248" s="6">
         <v>-15</v>
       </c>
@@ -16936,26 +16993,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="249" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C249" s="6"/>
       <c r="D249" s="8"/>
-      <c r="E249" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F249" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G249" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H249" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I249" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J249" s="6" t="b">
-        <v>1</v>
+      <c r="E249" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F249" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G249" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H249" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I249" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J249" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K249" s="6" t="b">
         <v>1</v>
@@ -17006,7 +17063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="250" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C250" s="6">
         <v>15</v>
       </c>
@@ -17078,7 +17135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="251" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C251" s="6"/>
       <c r="D251" s="8">
         <v>15</v>
@@ -17150,7 +17207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="252" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C252" s="6">
         <v>15</v>
       </c>
@@ -17224,7 +17281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="253" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C253" s="6">
         <v>-3</v>
       </c>
@@ -17298,7 +17355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="257" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C257" s="10" t="s">
         <v>418</v>
       </c>
@@ -17328,7 +17385,7 @@
       <c r="Y257" s="6"/>
       <c r="Z257" s="6"/>
     </row>
-    <row r="258" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="258" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C258" s="6" t="s">
         <v>53</v>
       </c>
@@ -17402,7 +17459,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="259" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="259" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C259" s="6" t="s">
         <v>55</v>
       </c>
@@ -17476,7 +17533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="260" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="260" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C260" s="7">
         <v>1</v>
       </c>
@@ -17550,7 +17607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="261" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C261" s="7">
         <v>-1</v>
       </c>
@@ -17624,7 +17681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="262" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C262" s="6">
         <v>0</v>
       </c>
@@ -17698,7 +17755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="263" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C263" s="6">
         <v>-15</v>
       </c>
@@ -17772,7 +17829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="264" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C264" s="6">
         <v>-15</v>
       </c>
@@ -17846,26 +17903,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="265" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C265" s="6"/>
       <c r="D265" s="8"/>
-      <c r="E265" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F265" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G265" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H265" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I265" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J265" s="6" t="b">
-        <v>1</v>
+      <c r="E265" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F265" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G265" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H265" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I265" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J265" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K265" s="6" t="b">
         <v>1</v>
@@ -17916,7 +17973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="266" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C266" s="6">
         <v>15</v>
       </c>
@@ -17988,7 +18045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="267" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C267" s="6"/>
       <c r="D267" s="8">
         <v>15</v>
@@ -18060,7 +18117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="268" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C268" s="6">
         <v>15</v>
       </c>
@@ -18134,7 +18191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="269" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C269" s="6">
         <v>-3</v>
       </c>
@@ -18208,7 +18265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="273" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C273" s="10" t="s">
         <v>441</v>
       </c>
@@ -18238,7 +18295,7 @@
       <c r="Y273" s="6"/>
       <c r="Z273" s="6"/>
     </row>
-    <row r="274" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="274" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C274" s="6" t="s">
         <v>53</v>
       </c>
@@ -18312,7 +18369,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="275" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="275" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C275" s="6" t="s">
         <v>55</v>
       </c>
@@ -18386,7 +18443,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="276" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C276" s="7">
         <v>1</v>
       </c>
@@ -18460,7 +18517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C277" s="7">
         <v>-1</v>
       </c>
@@ -18534,7 +18591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="278" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C278" s="6">
         <v>0</v>
       </c>
@@ -18608,7 +18665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="279" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C279" s="6">
         <v>-15</v>
       </c>
@@ -18682,7 +18739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C280" s="6">
         <v>-15</v>
       </c>
@@ -18756,26 +18813,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="281" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C281" s="6"/>
       <c r="D281" s="8"/>
-      <c r="E281" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F281" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G281" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H281" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I281" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J281" s="6" t="b">
-        <v>1</v>
+      <c r="E281" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F281" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G281" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H281" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I281" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J281" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K281" s="6" t="b">
         <v>1</v>
@@ -18826,7 +18883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="282" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C282" s="6">
         <v>15</v>
       </c>
@@ -18898,7 +18955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="283" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C283" s="6"/>
       <c r="D283" s="8">
         <v>15</v>
@@ -18970,7 +19027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="284" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C284" s="6">
         <v>15</v>
       </c>
@@ -19044,7 +19101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="285" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C285" s="6">
         <v>-3</v>
       </c>
@@ -19118,7 +19175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C289" s="10" t="s">
         <v>464</v>
       </c>
@@ -19148,7 +19205,7 @@
       <c r="Y289" s="6"/>
       <c r="Z289" s="6"/>
     </row>
-    <row r="290" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C290" s="6" t="s">
         <v>53</v>
       </c>
@@ -19222,7 +19279,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="291" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C291" s="6" t="s">
         <v>55</v>
       </c>
@@ -19296,7 +19353,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="292" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="292" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C292" s="7">
         <v>1</v>
       </c>
@@ -19370,7 +19427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="293" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C293" s="7">
         <v>-1</v>
       </c>
@@ -19444,7 +19501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="294" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C294" s="6">
         <v>0</v>
       </c>
@@ -19518,7 +19575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="295" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C295" s="6">
         <v>-15</v>
       </c>
@@ -19592,7 +19649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="296" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C296" s="6">
         <v>-15</v>
       </c>
@@ -19666,26 +19723,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="297" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C297" s="6"/>
       <c r="D297" s="8"/>
-      <c r="E297" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F297" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G297" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H297" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I297" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J297" s="6" t="b">
-        <v>1</v>
+      <c r="E297" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F297" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G297" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H297" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I297" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J297" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K297" s="6" t="b">
         <v>1</v>
@@ -19736,7 +19793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="298" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C298" s="6">
         <v>15</v>
       </c>
@@ -19808,7 +19865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="299" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C299" s="6"/>
       <c r="D299" s="8">
         <v>15</v>
@@ -19880,7 +19937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="300" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C300" s="6">
         <v>15</v>
       </c>
@@ -19954,7 +20011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="301" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C301" s="6">
         <v>-3</v>
       </c>
@@ -20028,7 +20085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="305" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C305" s="10" t="s">
         <v>487</v>
       </c>
@@ -20058,7 +20115,7 @@
       <c r="Y305" s="6"/>
       <c r="Z305" s="6"/>
     </row>
-    <row r="306" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="306" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C306" s="6" t="s">
         <v>53</v>
       </c>
@@ -20132,7 +20189,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="307" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="307" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C307" s="6" t="s">
         <v>55</v>
       </c>
@@ -20206,7 +20263,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="308" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="308" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C308" s="7">
         <v>1</v>
       </c>
@@ -20280,7 +20337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="309" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C309" s="7">
         <v>-1</v>
       </c>
@@ -20354,7 +20411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="310" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C310" s="6">
         <v>0</v>
       </c>
@@ -20428,7 +20485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="311" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C311" s="6">
         <v>-15</v>
       </c>
@@ -20502,7 +20559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="312" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C312" s="6">
         <v>-15</v>
       </c>
@@ -20576,26 +20633,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="313" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C313" s="6"/>
       <c r="D313" s="8"/>
-      <c r="E313" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F313" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G313" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H313" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I313" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J313" s="6" t="b">
-        <v>1</v>
+      <c r="E313" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F313" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G313" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H313" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I313" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J313" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K313" s="6" t="b">
         <v>1</v>
@@ -20646,7 +20703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="314" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C314" s="6">
         <v>15</v>
       </c>
@@ -20718,7 +20775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="315" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C315" s="6"/>
       <c r="D315" s="8">
         <v>15</v>
@@ -20790,7 +20847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="316" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C316" s="6">
         <v>15</v>
       </c>
@@ -20864,7 +20921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="317" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C317" s="6">
         <v>-3</v>
       </c>
@@ -20938,7 +20995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="321" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C321" s="10" t="s">
         <v>510</v>
       </c>
@@ -20968,7 +21025,7 @@
       <c r="Y321" s="6"/>
       <c r="Z321" s="6"/>
     </row>
-    <row r="322" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="322" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C322" s="6" t="s">
         <v>53</v>
       </c>
@@ -21042,7 +21099,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="323" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="323" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C323" s="6" t="s">
         <v>55</v>
       </c>
@@ -21116,7 +21173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="324" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="324" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C324" s="7">
         <v>1</v>
       </c>
@@ -21190,7 +21247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="325" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C325" s="7">
         <v>-1</v>
       </c>
@@ -21264,7 +21321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="326" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C326" s="6">
         <v>0</v>
       </c>
@@ -21338,7 +21395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="327" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C327" s="6">
         <v>-15</v>
       </c>
@@ -21412,7 +21469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="328" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C328" s="6">
         <v>-15</v>
       </c>
@@ -21486,26 +21543,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="329" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C329" s="6"/>
       <c r="D329" s="8"/>
-      <c r="E329" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F329" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G329" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H329" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I329" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J329" s="6" t="b">
-        <v>1</v>
+      <c r="E329" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F329" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G329" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H329" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I329" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J329" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K329" s="6" t="b">
         <v>1</v>
@@ -21556,7 +21613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="330" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C330" s="6">
         <v>15</v>
       </c>
@@ -21628,7 +21685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="331" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C331" s="6"/>
       <c r="D331" s="8">
         <v>15</v>
@@ -21700,7 +21757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="332" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C332" s="6">
         <v>15</v>
       </c>
@@ -21774,7 +21831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="333" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C333" s="6">
         <v>-3</v>
       </c>
@@ -21848,7 +21905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="337" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C337" s="10" t="s">
         <v>533</v>
       </c>
@@ -21878,7 +21935,7 @@
       <c r="Y337" s="6"/>
       <c r="Z337" s="6"/>
     </row>
-    <row r="338" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="338" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C338" s="6" t="s">
         <v>53</v>
       </c>
@@ -21952,7 +22009,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="339" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="339" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C339" s="6" t="s">
         <v>55</v>
       </c>
@@ -22026,7 +22083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="340" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="340" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C340" s="7">
         <v>1</v>
       </c>
@@ -22100,7 +22157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="341" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C341" s="7">
         <v>-1</v>
       </c>
@@ -22174,7 +22231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="342" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C342" s="6">
         <v>0</v>
       </c>
@@ -22248,7 +22305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="343" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C343" s="6">
         <v>-15</v>
       </c>
@@ -22322,7 +22379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="344" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C344" s="6">
         <v>-15</v>
       </c>
@@ -22396,26 +22453,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="345" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C345" s="6"/>
       <c r="D345" s="8"/>
-      <c r="E345" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F345" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G345" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H345" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I345" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J345" s="6" t="b">
-        <v>1</v>
+      <c r="E345" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F345" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G345" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H345" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I345" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J345" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K345" s="6" t="b">
         <v>1</v>
@@ -22466,7 +22523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="346" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C346" s="6">
         <v>15</v>
       </c>
@@ -22538,7 +22595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="347" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C347" s="6"/>
       <c r="D347" s="8">
         <v>15</v>
@@ -22610,7 +22667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="348" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C348" s="6">
         <v>15</v>
       </c>
@@ -22684,7 +22741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="349" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C349" s="6">
         <v>-3</v>
       </c>
@@ -22758,7 +22815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C353" s="10" t="s">
         <v>556</v>
       </c>
@@ -22788,7 +22845,7 @@
       <c r="Y353" s="6"/>
       <c r="Z353" s="6"/>
     </row>
-    <row r="354" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C354" s="6" t="s">
         <v>53</v>
       </c>
@@ -22862,7 +22919,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="355" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C355" s="6" t="s">
         <v>55</v>
       </c>
@@ -22936,7 +22993,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="356" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="356" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C356" s="7">
         <v>1</v>
       </c>
@@ -23010,7 +23067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="357" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C357" s="7">
         <v>-1</v>
       </c>
@@ -23084,7 +23141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="358" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C358" s="6">
         <v>0</v>
       </c>
@@ -23158,7 +23215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="359" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C359" s="6">
         <v>-15</v>
       </c>
@@ -23232,7 +23289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="360" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C360" s="6">
         <v>-15</v>
       </c>
@@ -23306,26 +23363,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="361" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C361" s="6"/>
       <c r="D361" s="8"/>
-      <c r="E361" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F361" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G361" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H361" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I361" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J361" s="6" t="b">
-        <v>1</v>
+      <c r="E361" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F361" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G361" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H361" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I361" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J361" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K361" s="6" t="b">
         <v>1</v>
@@ -23376,7 +23433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="362" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C362" s="6">
         <v>15</v>
       </c>
@@ -23448,7 +23505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="363" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C363" s="6"/>
       <c r="D363" s="8">
         <v>15</v>
@@ -23520,7 +23577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="364" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C364" s="6">
         <v>15</v>
       </c>
@@ -23594,7 +23651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="365" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C365" s="6">
         <v>-3</v>
       </c>
@@ -23668,7 +23725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="369" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C369" s="10" t="s">
         <v>579</v>
       </c>
@@ -23698,7 +23755,7 @@
       <c r="Y369" s="6"/>
       <c r="Z369" s="6"/>
     </row>
-    <row r="370" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="370" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C370" s="6" t="s">
         <v>53</v>
       </c>
@@ -23772,7 +23829,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="371" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="371" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C371" s="6" t="s">
         <v>55</v>
       </c>
@@ -23846,7 +23903,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="372" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="372" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C372" s="7">
         <v>1</v>
       </c>
@@ -23920,7 +23977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="373" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C373" s="7">
         <v>-1</v>
       </c>
@@ -23994,7 +24051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="374" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C374" s="6">
         <v>0</v>
       </c>
@@ -24068,7 +24125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="375" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C375" s="6">
         <v>-15</v>
       </c>
@@ -24142,7 +24199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="376" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C376" s="6">
         <v>-15</v>
       </c>
@@ -24216,26 +24273,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="377" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C377" s="6"/>
       <c r="D377" s="8"/>
-      <c r="E377" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F377" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G377" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H377" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I377" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J377" s="6" t="b">
-        <v>1</v>
+      <c r="E377" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F377" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G377" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H377" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I377" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J377" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="K377" s="6" t="b">
         <v>1</v>
@@ -24286,7 +24343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="378" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C378" s="6">
         <v>15</v>
       </c>
@@ -24358,7 +24415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="379" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C379" s="6"/>
       <c r="D379" s="8">
         <v>15</v>
@@ -24430,7 +24487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="380" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C380" s="6">
         <v>15</v>
       </c>
@@ -24504,7 +24561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="381" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C381" s="6">
         <v>-3</v>
       </c>

</xml_diff>